<commit_message>
accidently rolled back hayes whoops
</commit_message>
<xml_diff>
--- a/assets/FEATURES.xlsx
+++ b/assets/FEATURES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parkb\Documents\Repos\Sono\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{897B3A00-72C7-4CD2-9DB2-1A3A46323CEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F9CC60-98AA-4043-85EB-2F3DC14CEDBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1142,7 +1142,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
+      <selection pane="bottomLeft" activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3" x14ac:dyDescent="0.4"/>
@@ -8118,7 +8118,7 @@
         <v>0</v>
       </c>
       <c r="J61" s="31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K61" s="32" t="s">
         <v>0</v>
@@ -8170,7 +8170,7 @@
       </c>
       <c r="AA61" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>--+--++-----+---00--00000</v>
+        <v>--+--++-+---+---00--00000</v>
       </c>
     </row>
     <row r="62" spans="1:27" s="42" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
@@ -8202,7 +8202,7 @@
         <v>0</v>
       </c>
       <c r="J62" s="31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K62" s="32" t="s">
         <v>1</v>
@@ -8254,7 +8254,7 @@
       </c>
       <c r="AA62" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>--+--++--+--+---00--00000</v>
+        <v>--+--++-++--+---00--00000</v>
       </c>
     </row>
     <row r="63" spans="1:27" s="42" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
@@ -8454,7 +8454,7 @@
         <v>0</v>
       </c>
       <c r="J65" s="31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K65" s="32" t="s">
         <v>0</v>
@@ -8506,7 +8506,7 @@
       </c>
       <c r="AA65" s="40" t="str">
         <f t="shared" si="1"/>
-        <v>--+--++-----+-+-00--00000</v>
+        <v>--+--++-+---+-+-00--00000</v>
       </c>
     </row>
     <row r="66" spans="1:27" s="42" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
@@ -8538,7 +8538,7 @@
         <v>0</v>
       </c>
       <c r="J66" s="31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K66" s="32" t="s">
         <v>1</v>
@@ -8590,7 +8590,7 @@
       </c>
       <c r="AA66" s="40" t="str">
         <f t="shared" ref="AA66:AA97" si="2">_xlfn.CONCAT(B66:Z66)</f>
-        <v>--+--++--+--+-+-00--00000</v>
+        <v>--+--++-++--+-+-00--00000</v>
       </c>
     </row>
     <row r="67" spans="1:27" s="42" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
@@ -9294,7 +9294,7 @@
         <v>0</v>
       </c>
       <c r="J75" s="31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K75" s="32" t="s">
         <v>0</v>
@@ -9346,7 +9346,7 @@
       </c>
       <c r="AA75" s="40" t="str">
         <f t="shared" si="2"/>
-        <v>--+--++------00-00-++----</v>
+        <v>--+--++-+----00-00-++----</v>
       </c>
     </row>
     <row r="76" spans="1:27" s="42" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
@@ -9378,7 +9378,7 @@
         <v>0</v>
       </c>
       <c r="J76" s="31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K76" s="32" t="s">
         <v>1</v>
@@ -9430,7 +9430,7 @@
       </c>
       <c r="AA76" s="40" t="str">
         <f t="shared" si="2"/>
-        <v>--+--++--+---00-00-++----</v>
+        <v>--+--++-++---00-00-++----</v>
       </c>
     </row>
     <row r="77" spans="1:27" s="42" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
@@ -9462,7 +9462,7 @@
         <v>0</v>
       </c>
       <c r="J77" s="31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K77" s="32" t="s">
         <v>0</v>
@@ -9514,7 +9514,7 @@
       </c>
       <c r="AA77" s="40" t="str">
         <f t="shared" si="2"/>
-        <v>--+--++------00-00-+---+-</v>
+        <v>--+--++-+----00-00-+---+-</v>
       </c>
     </row>
     <row r="78" spans="1:27" s="42" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">
@@ -9546,7 +9546,7 @@
         <v>0</v>
       </c>
       <c r="J78" s="31" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K78" s="32" t="s">
         <v>1</v>
@@ -9598,7 +9598,7 @@
       </c>
       <c r="AA78" s="40" t="str">
         <f t="shared" si="2"/>
-        <v>--+--++--+---00-00-+---+-</v>
+        <v>--+--++-++---00-00-+---+-</v>
       </c>
     </row>
     <row r="79" spans="1:27" s="42" customFormat="1" ht="20.05" customHeight="1" x14ac:dyDescent="0.4">

</xml_diff>